<commit_message>
fix error and add noti, css, filter
</commit_message>
<xml_diff>
--- a/kms-fe/public/assets/excel/sample.xlsx
+++ b/kms-fe/public/assets/excel/sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin123456\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7643C4D1-A035-404E-86D6-BCD59C2C3EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9493D77-AAB1-4994-A137-B3FBF4C06D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data " sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t>ID</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>17 - Dự án học tập/Learning project</t>
-  </si>
-  <si>
-    <t>ClassID</t>
   </si>
   <si>
     <r>
@@ -185,13 +182,6 @@
     </r>
   </si>
   <si>
-    <t>Nhập mã Chương trình học áp dụng 
-(Ví dụ: SN,QT)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TeacherName </t>
-  </si>
-  <si>
     <t>TimeslotID</t>
   </si>
   <si>
@@ -232,9 +222,6 @@
   </si>
   <si>
     <t>6 - 12:00 - 14:00</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>??/??/????</t>
@@ -426,7 +413,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -625,11 +612,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -662,15 +675,6 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
@@ -697,6 +701,18 @@
     <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -917,8 +933,8 @@
   </sheetPr>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -930,11 +946,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.2" x14ac:dyDescent="0.5">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>55</v>
+      <c r="B1" s="21" t="s">
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -956,14 +972,14 @@
       <c r="D2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="34"/>
+      <c r="F2" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="29"/>
     </row>
     <row r="3" spans="1:11" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A3" s="2">
@@ -978,14 +994,14 @@
       <c r="D3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="37"/>
+      <c r="F3" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
     </row>
     <row r="4" spans="1:11" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A4" s="2">
@@ -1000,14 +1016,14 @@
       <c r="D4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="30"/>
+      <c r="F4" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="25"/>
     </row>
     <row r="5" spans="1:11" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
@@ -1022,19 +1038,19 @@
       <c r="D5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="30"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="25"/>
     </row>
     <row r="6" spans="1:11" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>15</v>
@@ -1042,21 +1058,21 @@
       <c r="D6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="37"/>
+      <c r="F6" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="32"/>
     </row>
     <row r="7" spans="1:11" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>17</v>
@@ -1064,14 +1080,14 @@
       <c r="D7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="40"/>
+      <c r="F7" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="35"/>
     </row>
     <row r="8" spans="1:11" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A8" s="2">
@@ -1084,7 +1100,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="22.8" x14ac:dyDescent="0.4">
@@ -1095,7 +1111,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D9" s="13"/>
     </row>
@@ -1107,7 +1123,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D10" s="13"/>
     </row>
@@ -1171,7 +1187,7 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D16" s="13"/>
     </row>
@@ -1184,10 +1200,10 @@
         <v>30</v>
       </c>
       <c r="D17" s="13"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="25" t="s">
-        <v>53</v>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="20" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="21" x14ac:dyDescent="0.35">
@@ -1206,13 +1222,13 @@
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D19" s="13"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="25" t="s">
-        <v>54</v>
+      <c r="F19" s="18"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="20" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1227,8 +1243,8 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1243,34 +1259,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A2" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>52</v>
+      <c r="A2" s="26"/>
+      <c r="B2" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>48</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="9"/>
@@ -1280,30 +1288,30 @@
     </row>
     <row r="3" spans="1:8" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="36" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="15"/>
@@ -1315,7 +1323,7 @@
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -1325,7 +1333,7 @@
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="36" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="15"/>
@@ -1337,7 +1345,7 @@
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -1347,7 +1355,7 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="36" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="15"/>
@@ -1359,7 +1367,7 @@
       <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -1369,7 +1377,7 @@
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="36" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="15"/>
@@ -1381,7 +1389,7 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -1391,8 +1399,8 @@
       <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
-        <v>49</v>
+      <c r="A12" s="36" t="s">
+        <v>46</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
@@ -1403,7 +1411,7 @@
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -1413,8 +1421,8 @@
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
-        <v>50</v>
+      <c r="A14" s="36" t="s">
+        <v>47</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -1425,7 +1433,7 @@
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
+      <c r="A15" s="37"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -1435,7 +1443,7 @@
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:8" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="36" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="15"/>
@@ -1447,7 +1455,7 @@
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
@@ -1457,7 +1465,7 @@
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="36" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="15"/>
@@ -1469,7 +1477,7 @@
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
+      <c r="A19" s="37"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
@@ -1479,7 +1487,7 @@
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="36" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="15"/>
@@ -1491,7 +1499,7 @@
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
@@ -1501,7 +1509,7 @@
       <c r="H21" s="8"/>
     </row>
     <row r="22" spans="1:8" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="15"/>
@@ -1513,7 +1521,7 @@
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
+      <c r="A23" s="37"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
@@ -1523,7 +1531,7 @@
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:8" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="36" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="15"/>
@@ -1535,7 +1543,7 @@
       <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
+      <c r="A25" s="38"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>

</xml_diff>